<commit_message>
Updaed evaluation with more information and better looking box plots
</commit_message>
<xml_diff>
--- a/results/genetic_eval.xlsx
+++ b/results/genetic_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSE6140\project\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23793E95-33F3-4949-9FCD-99E5D7405710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E36E7A-F276-4E9E-B815-FCFD331F0458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="genetic_eval" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">genetic_eval!$E$1:$G$1048558</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">genetic_eval!$C$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">genetic_eval!$C$2:$C$41</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">genetic_eval!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">genetic_eval!$B$2:$B$41</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Atlanta_QRTD!$D$1:$D$40</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">NYC_QRTD!$C$1:$C$40</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">NYC_QRTD!$C$1:$C$40</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">NYC_QRTD!$C$1:$C$40</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">NYC_QRTD!$C$1:$C$40</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Atlanta_QRTD!$D$1:$D$40</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">NYC_QRTD!$C$1:$C$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5039,7 +5032,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5101,7 +5094,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5144,7 +5137,7 @@
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
-      <cx:axis id="0">
+      <cx:axis id="0" hidden="1">
         <cx:catScaling gapWidth="1"/>
         <cx:tickLabels/>
       </cx:axis>
@@ -8615,16 +8608,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>578643</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>278605</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>21431</xdr:rowOff>
+      <xdr:rowOff>111918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>616743</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>316705</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>50006</xdr:rowOff>
+      <xdr:rowOff>140493</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8651,16 +8644,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>516731</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>21431</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>102394</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>290513</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30730</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>86794</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -8696,8 +8689,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3755231" y="1107281"/>
-              <a:ext cx="2364582" cy="3645694"/>
+              <a:off x="4410075" y="1369219"/>
+              <a:ext cx="2097655" cy="2880000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -16089,7 +16082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -16657,8 +16650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="G10:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>